<commit_message>
Fix the case where settable values are removed
</commit_message>
<xml_diff>
--- a/examples/blank.xlsx
+++ b/examples/blank.xlsx
@@ -382,12 +382,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <sheetData/>
+  <sheetData>
+    <row r="4" spans="1:1">
+      <c r="A4">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>